<commit_message>
Added field datatype validation
</commit_message>
<xml_diff>
--- a/src/templates/Format.xlsx
+++ b/src/templates/Format.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\var\www\flexphp\flex-generator\src\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Posts" sheetId="1" r:id="rId1"/>
     <sheet name="Comments" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -64,9 +59,6 @@
   </si>
   <si>
     <t>Title</t>
-  </si>
-  <si>
-    <t>interger</t>
   </si>
   <si>
     <t>PostId</t>
@@ -78,8 +70,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,7 +192,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -235,7 +227,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -412,23 +404,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -444,7 +436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -452,7 +444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -460,15 +452,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -476,7 +468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -491,16 +483,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -516,7 +508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -524,15 +516,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -540,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Added Constratins property in FormatProcess - WIP
</commit_message>
<xml_diff>
--- a/src/templates/Format.xlsx
+++ b/src/templates/Format.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6840" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6840"/>
   </bookViews>
   <sheets>
     <sheet name="Posts" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -83,6 +83,21 @@
   </si>
   <si>
     <t>Are</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>['required', 'type' =&gt; 'number']</t>
+  </si>
+  <si>
+    <t>['required' =&gt; false]</t>
+  </si>
+  <si>
+    <t>['required' =&gt; true, 'maxlength' =&gt; '255']</t>
+  </si>
+  <si>
+    <t>['required' =&gt; true, 'type' =&gt; 'textarea', 'length' =&gt; ['min' =&gt; 10, 'max' =&gt; 512]]</t>
   </si>
 </sst>
 </file>
@@ -430,55 +445,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -486,7 +516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -504,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated Constratins property in FormatProcess
</commit_message>
<xml_diff>
--- a/src/templates/Format.xlsx
+++ b/src/templates/Format.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Posts" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>['required' =&gt; true, 'type' =&gt; 'textarea', 'length' =&gt; ['min' =&gt; 10, 'max' =&gt; 512]]</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>required|min:3|max:256</t>
+  </si>
+  <si>
+    <t>required:true</t>
   </si>
 </sst>
 </file>
@@ -447,6 +456,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
@@ -472,115 +568,40 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>

</xml_diff>